<commit_message>
hot zone support and updated test_file
</commit_message>
<xml_diff>
--- a/Parameter experimentation data.xlsx
+++ b/Parameter experimentation data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceccarelli/Google Drive/REU/REU-Drone-Swarm-Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D75453E-12B8-E246-A0AD-A760D0743F46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC67072-1C66-254E-9054-AD6DF389CC06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{D9324A89-EF1B-2742-8BF0-637F7EBB650A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18560" windowHeight="18000" xr2:uid="{D9324A89-EF1B-2742-8BF0-637F7EBB650A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,12 +398,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,7 +1129,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>scatter</c:v>
+            <c:v>Scatter of Data Points</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1303,7 +1303,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>average line</c:v>
+            <c:v>Average Trendline</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1647,6 +1647,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5583,8 +5614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63A9D61-3F65-DF48-ABDD-6756A70D5827}">
   <dimension ref="B3:X56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:R19"/>
+    <sheetView tabSelected="1" topLeftCell="G27" zoomScale="215" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5704,7 +5735,7 @@
         <v>35.201000000000001</v>
       </c>
       <c r="L5" s="13"/>
-      <c r="N5" s="25">
+      <c r="N5" s="24">
         <v>0</v>
       </c>
       <c r="O5" s="3">
@@ -5827,7 +5858,7 @@
       <c r="P7" s="4">
         <v>8</v>
       </c>
-      <c r="Q7" s="26">
+      <c r="Q7" s="25">
         <v>52.45</v>
       </c>
       <c r="R7" s="16">
@@ -6548,86 +6579,86 @@
       </c>
     </row>
     <row r="21" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="H21" s="23" t="s">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="H21" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="N21" s="23" t="s">
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="N21" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="T21" s="23" t="s">
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="T21" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
     </row>
     <row r="22" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="H22" s="23" t="s">
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="H22" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="N22" s="23" t="s">
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="N22" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="T22" s="23" t="s">
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="T22" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="U22" s="23"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="23"/>
-      <c r="X22" s="23"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
     </row>
     <row r="23" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="23"/>
-      <c r="X23" s="23"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
     </row>
     <row r="24" spans="2:24" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="20"/>
@@ -6682,56 +6713,56 @@
       <c r="X25" s="20"/>
     </row>
     <row r="26" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="H26" s="23" t="s">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="H26" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="N26" s="23" t="s">
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="N26" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="T26" s="23" t="s">
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="T26" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="23"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="23"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="23"/>
-      <c r="X27" s="23"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="26"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B28" s="20"/>
@@ -6749,11 +6780,11 @@
       <c r="P28" s="20"/>
       <c r="Q28" s="20"/>
       <c r="R28" s="20"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="23"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
     </row>
     <row r="29" spans="2:24" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="20"/>
@@ -6771,11 +6802,11 @@
       <c r="P29" s="20"/>
       <c r="Q29" s="20"/>
       <c r="R29" s="20"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B30" s="20"/>
@@ -6793,11 +6824,11 @@
       <c r="P30" s="20"/>
       <c r="Q30" s="20"/>
       <c r="R30" s="20"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="23"/>
-      <c r="X30" s="23"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B31" s="20"/>
@@ -6822,37 +6853,37 @@
       <c r="X31" s="20"/>
     </row>
     <row r="44" spans="2:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N44" s="23" t="s">
+      <c r="N44" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26"/>
+      <c r="Q44" s="26"/>
+      <c r="R44" s="26"/>
     </row>
     <row r="45" spans="2:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
       <c r="H45" t="s">
         <v>18</v>
       </c>
-      <c r="N45" s="23"/>
-      <c r="O45" s="23"/>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="23"/>
+      <c r="N45" s="26"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="26"/>
+      <c r="R45" s="26"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B47" s="20"/>
@@ -6893,7 +6924,7 @@
       <c r="D51" s="3">
         <v>8</v>
       </c>
-      <c r="E51" s="24">
+      <c r="E51" s="23">
         <v>38.18</v>
       </c>
       <c r="F51" s="13"/>
@@ -6932,7 +6963,7 @@
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C54" s="3">
@@ -6971,7 +7002,7 @@
       <c r="D56" s="4">
         <v>8</v>
       </c>
-      <c r="E56" s="26">
+      <c r="E56" s="25">
         <v>52.45</v>
       </c>
       <c r="F56" s="16">
@@ -6981,20 +7012,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B26:F27"/>
+    <mergeCell ref="H26:L27"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B45:F46"/>
+    <mergeCell ref="N44:R45"/>
+    <mergeCell ref="B22:F23"/>
     <mergeCell ref="N21:R21"/>
     <mergeCell ref="N22:R23"/>
     <mergeCell ref="N26:R27"/>
     <mergeCell ref="T21:X21"/>
     <mergeCell ref="H21:L21"/>
     <mergeCell ref="H22:L23"/>
-    <mergeCell ref="B26:F27"/>
-    <mergeCell ref="H26:L27"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B45:F46"/>
-    <mergeCell ref="N44:R45"/>
     <mergeCell ref="T22:X23"/>
     <mergeCell ref="T26:X30"/>
-    <mergeCell ref="B22:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
data file and kmeans organization and optimization
</commit_message>
<xml_diff>
--- a/Parameter experimentation data.xlsx
+++ b/Parameter experimentation data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceccarelli/Google Drive/REU/REU-Drone-Swarm-Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC67072-1C66-254E-9054-AD6DF389CC06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64790528-15D3-D34A-86F7-8532027CA996}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18560" windowHeight="18000" xr2:uid="{D9324A89-EF1B-2742-8BF0-637F7EBB650A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18560" windowHeight="16440" xr2:uid="{D9324A89-EF1B-2742-8BF0-637F7EBB650A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -656,7 +656,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Average with lines</c:v>
+            <c:v>Average Trendline</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -795,7 +795,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> size</a:t>
+                  <a:t> Size</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -1001,6 +1001,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.1760684690009059E-2"/>
+          <c:y val="0.12436284119121846"/>
+          <c:w val="0.76358184664799233"/>
+          <c:h val="6.5398492789852325E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1129,7 +1170,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Scatter of Data Points</c:v>
+            <c:v>Scatter Plot</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1441,7 +1482,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> rate</a:t>
+                  <a:t> Rate</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -1761,7 +1802,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Between Runs Denominator Constant vs Runtime</a:t>
+              <a:t> Between Run vs Runtime</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1805,7 +1846,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>scatter</c:v>
+            <c:v>Scatter Plot</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1939,7 +1980,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>average line</c:v>
+            <c:v>Average Trendline</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2077,7 +2118,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Runs Denominator Constant</a:t>
+                  <a:t> Runs</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2283,6 +2324,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2411,7 +2483,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>scatter</c:v>
+            <c:v>Scatter Plot</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2554,7 +2626,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>average line</c:v>
+            <c:v>Average Trendline</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2898,6 +2970,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5281,13 +5384,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>4233</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>12699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>427566</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>35607</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5614,8 +5717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63A9D61-3F65-DF48-ABDD-6756A70D5827}">
   <dimension ref="B3:X56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G27" zoomScale="215" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="223" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7012,6 +7115,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="T21:X21"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="H22:L23"/>
+    <mergeCell ref="T22:X23"/>
+    <mergeCell ref="T26:X30"/>
     <mergeCell ref="B26:F27"/>
     <mergeCell ref="H26:L27"/>
     <mergeCell ref="B21:F21"/>
@@ -7021,11 +7129,6 @@
     <mergeCell ref="N21:R21"/>
     <mergeCell ref="N22:R23"/>
     <mergeCell ref="N26:R27"/>
-    <mergeCell ref="T21:X21"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="H22:L23"/>
-    <mergeCell ref="T22:X23"/>
-    <mergeCell ref="T26:X30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>